<commit_message>
Fixed selectors for Teams portion
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://independencegroup-my.sharepoint.com/personal/sanchit_kumar_igo_com_au/Documents/UiPath/NewTeamsTeam-Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2A5A0E25-4DD6-490A-9CC2-054902953D92}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9ADA8DC4-5857-4028-85F6-AD0B97B8590E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91C04A0A-71F2-452A-9A1F-615DB91DA6D0}"/>
   <bookViews>
     <workbookView xWindow="5900" yWindow="5280" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>https://admin.teams.microsoft.com</t>
   </si>
   <si>
-    <t>New-MSTeams-Team-a</t>
-  </si>
-  <si>
     <t>O365AdminCredentials</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>HelpDesk</t>
+  </si>
+  <si>
+    <t>New-MSTeams-Team</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -565,7 +565,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -594,19 +594,19 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>